<commit_message>
data updated on 2025-07-28 10:44:00.403219
</commit_message>
<xml_diff>
--- a/output/2025/scraped_data/Ministry of Health 2025.xlsx
+++ b/output/2025/scraped_data/Ministry of Health 2025.xlsx
@@ -6262,37 +6262,40 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Paola Pontoni</t>
+          <t>Bernardo Martorell</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Jefa Departamento de Reducción del Riesgo para Emergencias Sanitarias - SSP</t>
+          <t>Subsecretario de Redes Asistenciales</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/257591/805327</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/807448</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>AO001AW1854499</t>
+          <t>AO001AW1859806</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2025-06-09 04:30:00-04</t>
+          <t>2025-06-16 11:00:00-04</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Presencial</t>
+          <t>Videoconferencia</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Monjitas 689 piso 7 oficina 72</t>
+          <t>Será recibida en audiencia via teams, por Alison Morales, Asesora de Gabinete SUBSEREDES
+Id. de reunión: 259 600 552 338 
+Código de acceso: iC3JA9ck
+No se presentan</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -6302,17 +6305,19 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos., 
+Elaboración, tramitación, aprobación, modificación, derogación o rechazo de acuerdo, declaraciones o decisiones del Congreso Nacional o sus miembros incluídas comisiones.</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Soy medico urgenciologo, magister en emergencia y desastres. Me gustaría la asesoría de la jefa de departamento para el diseño de un proyecto que estoy llevando a cabo sobre manejo de múltiples victimas en hospitales.</t>
+          <t>CARGA LABORAL&lt;br /&gt;
+ELABORAR MESA TÉCNICA: AGRESIÓN Y RIESGOS DE TENS</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Rubén Nissin</t>
+          <t>Mireya Sanhueza</t>
         </is>
       </c>
       <c r="L126" t="inlineStr">
@@ -6323,82 +6328,29 @@
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr">
         <is>
-          <t>ruben nissin</t>
+          <t>COLEGIO NACIONAL DE TECNICOS EN ENFERMERIA DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>Paola Pontoni</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>Jefa Departamento de Reducción del Riesgo para Emergencias Sanitarias - SSP</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/257591/805541</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>AO001AW1815597</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>2025-04-09 17:30:00-04</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Presencial</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>oficina 1001 monjitas 565</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J127" t="inlineStr">
-        <is>
-          <t>Oportunidades de Mercado para la gestión climática bajo Art 6 del Acuerdo de París:&lt;br /&gt;
-(1) lista priorizada para tipología de proyectos; (2) línea del tiempo para lista priorizada; (3) apetito de proyectos en sector</t>
-        </is>
-      </c>
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr">
         <is>
-          <t>María Lucila Serra Lahunsembarne</t>
-        </is>
-      </c>
-      <c r="L127" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>South Pole Carbon Asset Management Ltd.</t>
-        </is>
-      </c>
-      <c r="N127" t="inlineStr">
-        <is>
-          <t>South Pole Carbon Asset Management Ltd.</t>
-        </is>
-      </c>
+          <t>Patricia Herrera Valenzuela</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr"/>
@@ -6413,104 +6365,32 @@
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr">
         <is>
-          <t>Rodrigo Bórquez</t>
-        </is>
-      </c>
-      <c r="L128" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>South Pole Carbon Asset Management Ltd.</t>
-        </is>
-      </c>
-      <c r="N128" t="inlineStr">
-        <is>
-          <t>South Pole Carbon Asset Management Ltd.</t>
-        </is>
-      </c>
+          <t>MANUEL LETELIER CUEVAS</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>Edith Carmen Ortiz Nuñez</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/786768</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>AO001AW1828916</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>2025-04-17 10:30:00-04</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>On line</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J129" t="inlineStr">
-        <is>
-          <t>Presentación de productos para detección y categorización de VPH, detección de VIH, Sífilis, HCV y HTLV&lt;br /&gt;
-&lt;br /&gt;
-Presentan equipos e insumos para la autotoma de examen de detección de VPH, a través de orina, permitiendo la amplificación y secuenciación de algunos genotipos. Presentan equipos e insumos para otros agentes: VIH, VHC, HTLV1, Sífilis. &lt;br /&gt;
-&lt;br /&gt;
-Se les sugiere reunión con ANACAN, y con redes asistenciales.&lt;br /&gt;
-&lt;br /&gt;
-Participan&lt;br /&gt;
-Dr. Leonardo Chanqueo Cornejo&lt;br /&gt;
-Carolina Peredo Courtier</t>
-        </is>
-      </c>
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr">
         <is>
-          <t>Andrés Fernández</t>
-        </is>
-      </c>
-      <c r="L129" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>Sociedad Comercial Mihovilovic Hnos. y Otro Ltda.</t>
-        </is>
-      </c>
-      <c r="N129" t="inlineStr">
-        <is>
-          <t>Sociedad Comercial Mihovilovic y Hnos y otro Limitada</t>
-        </is>
-      </c>
+          <t>RICARDO FUENTEALBA GUERRERO</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr"/>
@@ -6525,49 +6405,37 @@
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr">
         <is>
-          <t>Jorge Touma</t>
-        </is>
-      </c>
-      <c r="L130" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>Sociedad Comercial Mihovilovic Hnos. y Otro Ltda.</t>
-        </is>
-      </c>
-      <c r="N130" t="inlineStr">
-        <is>
-          <t>Sociedad Comercial Mihovilovic y Hnos y otro Limitada</t>
-        </is>
-      </c>
+          <t>SANDRA MELLA ORTIZ</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Edith Carmen Ortiz Nuñez</t>
+          <t>Bernardo Martorell</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
+          <t>Subsecretario de Redes Asistenciales</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/787885</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/803893</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>AO001AW1776471</t>
+          <t>AO001AW1847326</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2025-02-06 14:30:00-03</t>
+          <t>2025-06-02 11:00:00-04</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -6577,7 +6445,10 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>On line</t>
+          <t>lo recibirá Alison Morales Asesora del Subsecretario via Team
+Unirse a la reunión ahora 
+Id. de reunión: 290 165 488 188 5   lo recibió Alison Morales de forma presencial
+Código de acceso: Wm6RW9W6</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -6592,23 +6463,12 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Reunión de seguimiento lobby AO001AW1749073 en relación a la situación de Kaletra jarabe en programa VIH y una posible descontinuación.&lt;br /&gt;
-&lt;br /&gt;
-Se informa que se consultó al Comité asesor VIH pediátrico sobre existencia de alternativas terapéuticas, quienes señalaron y manifestaron la necesidad de mantener la disponibilidad de Kaletra® jarabe como parte del arsenal farmacológico para los niños y niñas que viven con VIH. &lt;br /&gt;
-Las alternativas disponibles en nuestro país pueden utilizarse a partir de los 40 kg, siendo inapropiados para la mayoría de los niños en crecimiento y no disponemos en Chile de su formulación en jarabes. Actualmente existen niños en control en que Kaletra® jarabe forma parte de su esquema de 2da línea y que no tienen el peso adecuado para optar a las alternativas disponibles.  &lt;br /&gt;
-&lt;br /&gt;
-Señalan que con estos antecedentes y teniendo claridad del requerimiento desde MINSAL realizarán gestiones para mantener la provisión de este producto en el país. &lt;br /&gt;
-&lt;br /&gt;
-Desde MINSAL se solicita informar sobre los avances de las gestiones por lo que se acuerda realizar una próxima reunión de seguimiento. &lt;br /&gt;
- &lt;br /&gt;
-Participan&lt;br /&gt;
-Leonardo Chanqueo Cornejo&lt;br /&gt;
-María Teresa Silva</t>
+          <t>Buenos solicito expresamente un audiencia con esta autoridad, para manifestar personalmente mi reclamo y con documentos en mano , lo que estoy reclamando en forma reiterada antes los diferentes organismos de salud y ala vez solicito que no se me derive nuevamente con otra persona , ya que con la persona que me derivaron anteriormente no he conseguido nada , ya que ella en aquella oportunidad se contactó con una persona del servicio de salud Ñuble y durante esta semana fuí a preguntarle que había sucedido con las gestiones que le habían solicitado desde el ministerio de salud desde Santiago, y la Respuesta INSÓLITA que me dio fue, Que HABÍA QUÉ MATAR AÚN PAR De PACIENTE PARA Que Yo pudiera ser atendido, lo cual creo que no corresponde ese tipo de respuesta sobre todo de un funcionario de dicho dpt de salud, por que ellos están Pará ayudar a tratar de solucionar los diferentes problemas que se le presenten a los pacientes y no dar ése tipo de respuesta</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>María Pons</t>
+          <t>Marcelo Chavarria Fuentes</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
@@ -6619,24 +6479,71 @@
       <c r="M131" t="inlineStr"/>
       <c r="N131" t="inlineStr">
         <is>
-          <t>Abbvie Ltda</t>
+          <t>Marcelo Chavarria fuentes</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr"/>
-      <c r="B132" t="inlineStr"/>
-      <c r="C132" t="inlineStr"/>
-      <c r="D132" t="inlineStr"/>
-      <c r="E132" t="inlineStr"/>
-      <c r="F132" t="inlineStr"/>
-      <c r="G132" t="inlineStr"/>
-      <c r="H132" t="inlineStr"/>
-      <c r="I132" t="inlineStr"/>
-      <c r="J132" t="inlineStr"/>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Bernardo Martorell</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Subsecretario de Redes Asistenciales</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/803892</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>AO001AW1831450</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>2025-06-02 11:00:00-04</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Tema: Lobby 1831450  ACTI A.G. 
+Hora: 2 jun 2025 11:00 p. m. Santiago
+Únase a la reunión de Zoom
+https://us02web.zoom.us/j/85980392427?pwd=UVg6NReDoYodcykhepWQsl99CWD9CD.1
+ID de reunión: 859 8039 2427
+Código de acceso: 755281    lo recibió Vanessa Diaz</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>La Asociación Chilena de Empresas de Tecnologías de Información A.G., a través de su Mesa de Salud, solicita poder reunirse con el señor Bernardo Martorell, Subsecretario de Redes Asistenciales, para conversar sobre de Ley Interoperabilidad de Fichas Clínicas y ofrecer la disposición desde ACTI a colaborar en esa instancia.&lt;br /&gt;
+&lt;br /&gt;
+A la reunión asistirán los señores Martín Kozak y René Prieto, Presidente y Vicepresidente de la Mesa de Salud de ACTI.</t>
+        </is>
+      </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Claudio Silva</t>
+          <t>Leandro Martin Kozak</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
@@ -6644,80 +6551,31 @@
           <t>Gestor de intereses</t>
         </is>
       </c>
-      <c r="M132" t="inlineStr"/>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>Intersysyems Chile Ltda</t>
+        </is>
+      </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>Abbvie Ltda</t>
+          <t>ASOCIACIÓN CHILENA DE EMPRESAS DE TECNOLOGÍAS DE INFORMACIÓN A.G. - ACTI A.G.</t>
         </is>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>Edith Carmen Ortiz Nuñez</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/780151</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>AO001AW1749073</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>2025-01-22 12:30:00-03</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>Presencial</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>Oficina Programa de VIH</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J133" t="inlineStr">
-        <is>
-          <t>Situación lopinavir/ritonavir solución oral en programa pediátrico VIH&lt;br /&gt;
-&lt;br /&gt;
-Señalan que debido a nuevas alternativas terapéuticas ha disminuido su demanda a nivel mundial, lo que se ha traducido en una discontinuación en la producción del producto. &lt;br /&gt;
-Actualmente tiene contrato vigente con CENABAST hasta diciembre 2025. Para el 2026 existe riesgo de descontinuación. &lt;br /&gt;
-Señalan que en caso de que MINSAL requiera mantener disponible este producto en el país podrían hacer las gestiones pertinentes para ello, considerando las dificultades que se pueden presentar. &lt;br /&gt;
-Desde el Depto VIH se plantea que es necesario disponer de esta presentación como una alternativa en tratamiento de rescate cuando existe resistencia a antirretrovirales. Lopinavir/ritonavir es la única alternativa que existe para estos casos en niños menores a &lt; 40 kilos. Igualmente se hará la consulta al Comité asesor VIH pediátrico para tener certeza que no existen otras alternativas terapéuticas en esta situación.&lt;br /&gt;
-Se acuerda realizar una próxima reunión de seguimiento para informar si se requiere mantener la disponibilidad de lopinavir/ritonavir solución en el país y realizar las gestiones correspondientes para ello. &lt;br /&gt;
-&lt;br /&gt;
-Asisten&lt;br /&gt;
-&lt;br /&gt;
-Dr. leonardo Chanqueo   Jefe Programa de VIH&lt;br /&gt;
-Sra. María Teresa Silva Profesional Programa de VIH&lt;br /&gt;
-Sra. María Pons&lt;br /&gt;
-Sr. Claudio Silva</t>
-        </is>
-      </c>
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr">
         <is>
-          <t>María Pons</t>
+          <t>René Prieto</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
@@ -6728,24 +6586,70 @@
       <c r="M133" t="inlineStr"/>
       <c r="N133" t="inlineStr">
         <is>
-          <t>Abbvie Ltda</t>
+          <t>ASOCIACIÓN CHILENA DE EMPRESAS DE TECNOLOGÍAS DE INFORMACIÓN A.G. - ACTI A.G.</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr"/>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr"/>
-      <c r="F134" t="inlineStr"/>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
-      <c r="I134" t="inlineStr"/>
-      <c r="J134" t="inlineStr"/>
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Bernardo Martorell</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Subsecretario de Redes Asistenciales</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800580</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>AO001AW1840794</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>2025-05-23 15:00:00-04</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>lo recibira Alison Morales asesora del Subsecretario de Redes ,  
+via TEAMS
+Unirse a la reunión ahora
+Id. de reunión: 268 496 198 113
+Código de acceso: vB2sX98b</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>1.- Implementación y funcionamiento del Ges 85 en APS y red de salud a nivel nacional, &lt;br /&gt;
+2.- Consultar si existe Protocolo en Atención Terciaria para hospitalización de personas con Alzheimer y Otras Demencias y personas con discapacidad, dependencia, o alguna condición.&lt;br /&gt;
+3.- Implementación ley 21.380 relacionada a las personas cuidadoras y exámenes médicos,</t>
+        </is>
+      </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>Claudio Silva</t>
+          <t>Paola Reyes</t>
         </is>
       </c>
       <c r="L134" t="inlineStr">
@@ -6756,70 +6660,24 @@
       <c r="M134" t="inlineStr"/>
       <c r="N134" t="inlineStr">
         <is>
-          <t>Abbvie Ltda</t>
+          <t>Paola Reyes Franco</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Carolina Neira</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Jefa (S) Departamento Enfermedades No Transmisibles</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/278283/792465</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>AO001AW1794134</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>2025-05-09 15:00:00-04</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>________________________________________________________________________________
-Microsoft Teams ¿Necesita ayuda? 
-Unirse a la reunión ahora 
-Id. de reunión: 228 396 235 533 1 
-Código de acceso: 5Nk3zg7Q 
-________________________________________</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
-        <is>
-          <t>0 horas, 15 minutos</t>
-        </is>
-      </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>Celebración, modificación o terminación a cualquier título, de contratos que realicen los sujetos pasivos y que sean necesarios para su funcionamiento., 
-Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J135" t="inlineStr">
-        <is>
-          <t>No se presenta a audiencia de Lobby.</t>
-        </is>
-      </c>
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr">
         <is>
-          <t>Juan Ríos</t>
+          <t>Constanza Gonzalez</t>
         </is>
       </c>
       <c r="L135" t="inlineStr">
@@ -6830,7 +6688,7 @@
       <c r="M135" t="inlineStr"/>
       <c r="N135" t="inlineStr">
         <is>
-          <t>Marcela Cofré Cervera</t>
+          <t>Constanza Gonzalez</t>
         </is>
       </c>
     </row>
@@ -6847,30 +6705,27 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/807448</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/796246</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>AO001AW1859806</t>
+          <t>AO001AW1824856</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2025-06-16 11:00:00-04</t>
+          <t>2025-05-16 08:30:00-04</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Videoconferencia</t>
+          <t>Presencial</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Será recibida en audiencia via teams, por Alison Morales, Asesora de Gabinete SUBSEREDES
-Id. de reunión: 259 600 552 338 
-Código de acceso: iC3JA9ck
-No se presentan</t>
+          <t>lo recibirá el Dr Bernardo Martorell, Subsecretario de Redes Asistenciales en Mac Iver 541 piso 2</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -6880,19 +6735,17 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos., 
-Elaboración, tramitación, aprobación, modificación, derogación o rechazo de acuerdo, declaraciones o decisiones del Congreso Nacional o sus miembros incluídas comisiones.</t>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>CARGA LABORAL&lt;br /&gt;
-ELABORAR MESA TÉCNICA: AGRESIÓN Y RIESGOS DE TENS</t>
+          <t>Dar a conocer al Subsecretario trabajo de FALP con pacientes del Sistema Público de Salud</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Mireya Sanhueza</t>
+          <t>Cristian Enrique Ayala Munita</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
@@ -6900,10 +6753,14 @@
           <t>Gestor de intereses</t>
         </is>
       </c>
-      <c r="M136" t="inlineStr"/>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>Fundación Arturo Lopez Perez</t>
+        </is>
+      </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>COLEGIO NACIONAL DE TECNICOS EN ENFERMERIA DE CHILE</t>
+          <t>FUNDACION ARTURO LOPEZ PEREZ</t>
         </is>
       </c>
     </row>
@@ -6920,52 +6777,186 @@
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr">
         <is>
-          <t>Patricia Herrera Valenzuela</t>
-        </is>
-      </c>
-      <c r="L137" t="inlineStr"/>
-      <c r="M137" t="inlineStr"/>
-      <c r="N137" t="inlineStr"/>
+          <t>Vladimir Pizarro</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>SERVICIO SALUD METROPOLITANO OCCIDENTE</t>
+        </is>
+      </c>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>FUNDACION ARTURO LOPEZ PEREZ</t>
+        </is>
+      </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr"/>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" t="inlineStr"/>
-      <c r="D138" t="inlineStr"/>
-      <c r="E138" t="inlineStr"/>
-      <c r="F138" t="inlineStr"/>
-      <c r="G138" t="inlineStr"/>
-      <c r="H138" t="inlineStr"/>
-      <c r="I138" t="inlineStr"/>
-      <c r="J138" t="inlineStr"/>
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Bernardo Martorell</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Subsecretario de Redes Asistenciales</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800575</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>AO001AW1824783</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:30:00-04</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>lo recibira via TEEM Alyson Morales Asesora del Gabinete  
+se adjunta TEEMUnirse a la reunión ahora 
+Id. de reunión: 291 166 863 411 9 
+Código de acceso: KU78PQ9o</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>MINUTA REUNIÓN SUBSECRETARIO DE REDES ASISTENCIALES. &lt;br /&gt;
+&lt;br /&gt;
+EL DEPARTAMENTO DE SALUD DE PAIHUANO, ES UN DEPARTAMENTO CUYO APORTE ES DE MENOS DE 5 MIL HABITANTES, POR ELLO ES CONSIDERANDO COMO COMUNA DE COSTO FPOR LO QUE EL APORTE MENSUAL ES VÍA PRCAPITA   DE PARTE DEL MINSAL POR CASI 43 MILLONES DE PESOS., RECUSO QUE ES UTILIZADO EN SU TOTALIDAD PARA LA CANCELACIÓN DE RECURSO HUMANO.&lt;br /&gt;
+EL APORTE MNICIPAL A SU VEZ AL DEPARTAMENTO DE SALUD ES DE ALREDEDOR DEL 55% DEL PRESUPUESTO DE SALUD ANUAL. ESE ES UN GRAN COMPROMISO HACIA EL DEPARTAMENTO ADQUIRIDO POR AÑOS   PERO QUE NO PUEDE SER MAYOR POR TODOS LOS COMPROMISOS QUE EL MUNICIPIO DEBE CUMPLIR CON LOS OTROS DEPARTAMENTOS. &lt;br /&gt;
+DE ESA FORMA SE HAN IDO GENERANDO BRECHAS., BRECHAS D TODO TIPO, QUE SE HAN TRATADO DE DISMINUIR REALIZANDO GESTIONES EN DIVERSOS NIVELES, PERO NINGUNA HA TENIDO RESULTADOS., POR DICHA RAZÓN SOLICITAMOS SU APOYO EN LOS SIGUIENTS REQUERIMIENTOS:&lt;br /&gt;
+1.- El DEAPRTAMENTO DE SALUD, CONTRATA SUS SERVICIOS DE EXÁMENES DE LABORATORIO CON EL HOSPITAL DE VICUÑA, POR MOTIVOS PRESUPUESTARIOS NO HA SIDO POSIBLE CANCELAR  DICHO SERVICIO, AL DÍA DE HOY EXISTE UNA DEUDA ACUMULADA DE 125 MILLONES DE PESOS, QUE NO PODEMOS CANCELAR , SOLICITAMOS QUE  SE PUEDA INTERVENIR EN APROBAR UN PROYECTO AGL  PARA LA  CANCELACIÓN  DE LOS EXÁMENES DE LABORATORIO  O LA RECONVERSIÓN DE RECURSOS , YA SEA RENDIR  RECURSO HUMANO DE DOTACIÓN  MUNICIPAL DE SALUD Y PARA PODER CONTAR DE ESA MANERA CON  EL DINERO DISPONIBLE PARA LA CANCELACIÓN DEL LABORATOTRIO  U  OTRA VIA POSIBLE DE COLABORACIÓN.&lt;br /&gt;
+2.-  SE REQUIERE EL APOYO DEL MINISTERIO DE SALUD EN EL PROCESO DE ACREDITACIÓN EN CALIDAD, 20 MILLONES PARA LA INSCRIPCIÓN EN EL PROCESO Y MEJORAS INTERNAS QUE SE REQUIERAN REALIZAR EN POSTAS Y CESFAM PARA AFRONTAR DICHO PROCESO.&lt;br /&gt;
+3.- ADQUISICIÓN DE CAMIONETA PARA RONDAS ASISITENCIALES Y OTRAS PRESTACIONES.&lt;br /&gt;
+4.- APROBACIÓN DE AGL Y PMI&lt;br /&gt;
+5.- CANCELACIÓN DE RECURSO HUMANO DE DOTACIÓN PARA LIBERACIÓN DE PRESUPUESTO&lt;br /&gt;
+&lt;br /&gt;
+                                                             AGRADECIDOS DEL APOYO.</t>
+        </is>
+      </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>MANUEL LETELIER CUEVAS</t>
-        </is>
-      </c>
-      <c r="L138" t="inlineStr"/>
-      <c r="M138" t="inlineStr"/>
-      <c r="N138" t="inlineStr"/>
+          <t>Mildred Varela</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>MUNICIPALIDAD DE PAIHUANO</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>ILUSTRE MUNICIPALIDAD DE PAIHUANO</t>
+        </is>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr"/>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr"/>
-      <c r="E139" t="inlineStr"/>
-      <c r="F139" t="inlineStr"/>
-      <c r="G139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
-      <c r="I139" t="inlineStr"/>
-      <c r="J139" t="inlineStr"/>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Bernardo Martorell</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Subsecretario de Redes Asistenciales</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800576</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>AO001AW1825815</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:30:00-04</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>lo recibirá en audiencia Alyson Morales Asesora del Gabinete 
+ Via TEEMUnirse a la reunión ahora 
+Id. de reunión: 264 303 737 002 5 
+Código de acceso: De6hw7fe</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>Presentar los Círculos de Escucha como una tecnología social y práctica grupal de bienestar recogida en el REM, y a Corporación Escuchar, como OSFL con 10 años de experiencia en instalar Círculos de Escucha y formar monitoras/es para ello. &lt;br /&gt;
+Proponemos usar Círculos de Escucha para:&lt;br /&gt;
+- promover la participación ciudadana en salud.&lt;br /&gt;
+- promover bienestar y salud comunitaria a bajo costo, en base a la comunidad.&lt;br /&gt;
+- construir y/o desarrollar vínculos saludables para potenciar las comunidades.&lt;br /&gt;
+- levantar, relevar, difundir y potenciar los activos comunitarios territoriales.</t>
+        </is>
+      </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>RICARDO FUENTEALBA GUERRERO</t>
-        </is>
-      </c>
-      <c r="L139" t="inlineStr"/>
+          <t>Verónica Virgilio</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
       <c r="M139" t="inlineStr"/>
-      <c r="N139" t="inlineStr"/>
+      <c r="N139" t="inlineStr">
+        <is>
+          <t>Corporación Escuchar</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr"/>
@@ -6980,12 +6971,20 @@
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr">
         <is>
-          <t>SANDRA MELLA ORTIZ</t>
-        </is>
-      </c>
-      <c r="L140" t="inlineStr"/>
+          <t>Yasna Nanjari</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
       <c r="M140" t="inlineStr"/>
-      <c r="N140" t="inlineStr"/>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>Corporación Escuchar</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -7000,17 +6999,17 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/803893</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800572</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>AO001AW1847326</t>
+          <t>AO001AW1815203</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>2025-06-02 11:00:00-04</t>
+          <t>2025-05-09 11:00:00-04</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -7020,10 +7019,11 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>lo recibirá Alison Morales Asesora del Subsecretario via Team
+          <t>lo recibirá en reunión  Alyson Morales asesora del Gabinete  por TEEM
+Microsoft Teams 
 Unirse a la reunión ahora 
-Id. de reunión: 290 165 488 188 5   lo recibió Alison Morales de forma presencial
-Código de acceso: Wm6RW9W6</t>
+Id. de reunión: 285 804 262 906 4 
+Código de acceso: ch7HJ6qQ</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -7038,12 +7038,12 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>Buenos solicito expresamente un audiencia con esta autoridad, para manifestar personalmente mi reclamo y con documentos en mano , lo que estoy reclamando en forma reiterada antes los diferentes organismos de salud y ala vez solicito que no se me derive nuevamente con otra persona , ya que con la persona que me derivaron anteriormente no he conseguido nada , ya que ella en aquella oportunidad se contactó con una persona del servicio de salud Ñuble y durante esta semana fuí a preguntarle que había sucedido con las gestiones que le habían solicitado desde el ministerio de salud desde Santiago, y la Respuesta INSÓLITA que me dio fue, Que HABÍA QUÉ MATAR AÚN PAR De PACIENTE PARA Que Yo pudiera ser atendido, lo cual creo que no corresponde ese tipo de respuesta sobre todo de un funcionario de dicho dpt de salud, por que ellos están Pará ayudar a tratar de solucionar los diferentes problemas que se le presenten a los pacientes y no dar ése tipo de respuesta</t>
+          <t>Vulneración de derechos a paciente Albero Jesús Garrido Pérez, en atenciones brindadas.</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>Marcelo Chavarria Fuentes</t>
+          <t>Alberto Garrido</t>
         </is>
       </c>
       <c r="L141" t="inlineStr">
@@ -7054,7 +7054,7 @@
       <c r="M141" t="inlineStr"/>
       <c r="N141" t="inlineStr">
         <is>
-          <t>Marcelo Chavarria fuentes</t>
+          <t>Gabriela Calderón Álvarez</t>
         </is>
       </c>
     </row>
@@ -7071,32 +7071,27 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/803892</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/796230</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>AO001AW1831450</t>
+          <t>AO001AW1822942</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2025-06-02 11:00:00-04</t>
+          <t>2025-05-08 11:30:00-04</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Videoconferencia</t>
+          <t>Presencial</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Tema: Lobby 1831450  ACTI A.G. 
-Hora: 2 jun 2025 11:00 p. m. Santiago
-Únase a la reunión de Zoom
-https://us02web.zoom.us/j/85980392427?pwd=UVg6NReDoYodcykhepWQsl99CWD9CD.1
-ID de reunión: 859 8039 2427
-Código de acceso: 755281    lo recibió Vanessa Diaz</t>
+          <t>Mac Iver 541 piso 2 Ministerio de Salud, contacto Doris González 225740370</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -7106,19 +7101,17 @@
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
         </is>
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>La Asociación Chilena de Empresas de Tecnologías de Información A.G., a través de su Mesa de Salud, solicita poder reunirse con el señor Bernardo Martorell, Subsecretario de Redes Asistenciales, para conversar sobre de Ley Interoperabilidad de Fichas Clínicas y ofrecer la disposición desde ACTI a colaborar en esa instancia.&lt;br /&gt;
-&lt;br /&gt;
-A la reunión asistirán los señores Martín Kozak y René Prieto, Presidente y Vicepresidente de la Mesa de Salud de ACTI.</t>
+          <t>Presentar Exposalud 2025 a realizarse 1,2 y 3 de diciembre en Espacio Riesco, con la finalidad de mostrar la plataforma público privada que es y como es que esto favorece la comunicación en el área de Salud. Es necesario que sepa las gestiones que realizamos para contar con su acuerdo y verificar que nos aliniemos en el trabajo a realizar.</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>Leandro Martin Kozak</t>
+          <t>Andrea Buzzetti</t>
         </is>
       </c>
       <c r="L142" t="inlineStr">
@@ -7128,12 +7121,12 @@
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>Intersysyems Chile Ltda</t>
+          <t>FRESENIUS KABI</t>
         </is>
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>ASOCIACIÓN CHILENA DE EMPRESAS DE TECNOLOGÍAS DE INFORMACIÓN A.G. - ACTI A.G.</t>
+          <t>andrea buzzetti</t>
         </is>
       </c>
     </row>
@@ -7150,7 +7143,7 @@
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr">
         <is>
-          <t>René Prieto</t>
+          <t>Miguel Berrios Momberg</t>
         </is>
       </c>
       <c r="L143" t="inlineStr">
@@ -7161,7 +7154,7 @@
       <c r="M143" t="inlineStr"/>
       <c r="N143" t="inlineStr">
         <is>
-          <t>ASOCIACIÓN CHILENA DE EMPRESAS DE TECNOLOGÍAS DE INFORMACIÓN A.G. - ACTI A.G.</t>
+          <t>Miguel Berrios</t>
         </is>
       </c>
     </row>
@@ -7178,17 +7171,17 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800580</t>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/787881</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>AO001AW1840794</t>
+          <t>AO001AW1822390</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>2025-05-23 15:00:00-04</t>
+          <t>2025-04-25 10:00:00-04</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -7198,11 +7191,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>lo recibira Alison Morales asesora del Subsecretario de Redes ,  
-via TEAMS
-Unirse a la reunión ahora
-Id. de reunión: 268 496 198 113
-Código de acceso: vB2sX98b</t>
+          <t>se encomendó a la División de Inversiones lo recibió  Adrian Peña  25 abril</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -7212,574 +7201,10 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
-        <is>
-          <t>1.- Implementación y funcionamiento del Ges 85 en APS y red de salud a nivel nacional, &lt;br /&gt;
-2.- Consultar si existe Protocolo en Atención Terciaria para hospitalización de personas con Alzheimer y Otras Demencias y personas con discapacidad, dependencia, o alguna condición.&lt;br /&gt;
-3.- Implementación ley 21.380 relacionada a las personas cuidadoras y exámenes médicos,</t>
-        </is>
-      </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>Paola Reyes</t>
-        </is>
-      </c>
-      <c r="L144" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M144" t="inlineStr"/>
-      <c r="N144" t="inlineStr">
-        <is>
-          <t>Paola Reyes Franco</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr"/>
-      <c r="B145" t="inlineStr"/>
-      <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr"/>
-      <c r="E145" t="inlineStr"/>
-      <c r="F145" t="inlineStr"/>
-      <c r="G145" t="inlineStr"/>
-      <c r="H145" t="inlineStr"/>
-      <c r="I145" t="inlineStr"/>
-      <c r="J145" t="inlineStr"/>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>Constanza Gonzalez</t>
-        </is>
-      </c>
-      <c r="L145" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M145" t="inlineStr"/>
-      <c r="N145" t="inlineStr">
-        <is>
-          <t>Constanza Gonzalez</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/796246</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>AO001AW1824856</t>
-        </is>
-      </c>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>2025-05-16 08:30:00-04</t>
-        </is>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>Presencial</t>
-        </is>
-      </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>lo recibirá el Dr Bernardo Martorell, Subsecretario de Redes Asistenciales en Mac Iver 541 piso 2</t>
-        </is>
-      </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J146" t="inlineStr">
-        <is>
-          <t>Dar a conocer al Subsecretario trabajo de FALP con pacientes del Sistema Público de Salud</t>
-        </is>
-      </c>
-      <c r="K146" t="inlineStr">
-        <is>
-          <t>Cristian Enrique Ayala Munita</t>
-        </is>
-      </c>
-      <c r="L146" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M146" t="inlineStr">
-        <is>
-          <t>Fundación Arturo Lopez Perez</t>
-        </is>
-      </c>
-      <c r="N146" t="inlineStr">
-        <is>
-          <t>FUNDACION ARTURO LOPEZ PEREZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr"/>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-      <c r="D147" t="inlineStr"/>
-      <c r="E147" t="inlineStr"/>
-      <c r="F147" t="inlineStr"/>
-      <c r="G147" t="inlineStr"/>
-      <c r="H147" t="inlineStr"/>
-      <c r="I147" t="inlineStr"/>
-      <c r="J147" t="inlineStr"/>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>Vladimir Pizarro</t>
-        </is>
-      </c>
-      <c r="L147" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M147" t="inlineStr">
-        <is>
-          <t>SERVICIO SALUD METROPOLITANO OCCIDENTE</t>
-        </is>
-      </c>
-      <c r="N147" t="inlineStr">
-        <is>
-          <t>FUNDACION ARTURO LOPEZ PEREZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800575</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>AO001AW1824783</t>
-        </is>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>2025-05-13 09:30:00-04</t>
-        </is>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>Presencial</t>
-        </is>
-      </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>lo recibira via TEEM Alyson Morales Asesora del Gabinete  
-se adjunta TEEMUnirse a la reunión ahora 
-Id. de reunión: 291 166 863 411 9 
-Código de acceso: KU78PQ9o</t>
-        </is>
-      </c>
-      <c r="H148" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J148" t="inlineStr">
-        <is>
-          <t>MINUTA REUNIÓN SUBSECRETARIO DE REDES ASISTENCIALES. &lt;br /&gt;
-&lt;br /&gt;
-EL DEPARTAMENTO DE SALUD DE PAIHUANO, ES UN DEPARTAMENTO CUYO APORTE ES DE MENOS DE 5 MIL HABITANTES, POR ELLO ES CONSIDERANDO COMO COMUNA DE COSTO FPOR LO QUE EL APORTE MENSUAL ES VÍA PRCAPITA   DE PARTE DEL MINSAL POR CASI 43 MILLONES DE PESOS., RECUSO QUE ES UTILIZADO EN SU TOTALIDAD PARA LA CANCELACIÓN DE RECURSO HUMANO.&lt;br /&gt;
-EL APORTE MNICIPAL A SU VEZ AL DEPARTAMENTO DE SALUD ES DE ALREDEDOR DEL 55% DEL PRESUPUESTO DE SALUD ANUAL. ESE ES UN GRAN COMPROMISO HACIA EL DEPARTAMENTO ADQUIRIDO POR AÑOS   PERO QUE NO PUEDE SER MAYOR POR TODOS LOS COMPROMISOS QUE EL MUNICIPIO DEBE CUMPLIR CON LOS OTROS DEPARTAMENTOS. &lt;br /&gt;
-DE ESA FORMA SE HAN IDO GENERANDO BRECHAS., BRECHAS D TODO TIPO, QUE SE HAN TRATADO DE DISMINUIR REALIZANDO GESTIONES EN DIVERSOS NIVELES, PERO NINGUNA HA TENIDO RESULTADOS., POR DICHA RAZÓN SOLICITAMOS SU APOYO EN LOS SIGUIENTS REQUERIMIENTOS:&lt;br /&gt;
-1.- El DEAPRTAMENTO DE SALUD, CONTRATA SUS SERVICIOS DE EXÁMENES DE LABORATORIO CON EL HOSPITAL DE VICUÑA, POR MOTIVOS PRESUPUESTARIOS NO HA SIDO POSIBLE CANCELAR  DICHO SERVICIO, AL DÍA DE HOY EXISTE UNA DEUDA ACUMULADA DE 125 MILLONES DE PESOS, QUE NO PODEMOS CANCELAR , SOLICITAMOS QUE  SE PUEDA INTERVENIR EN APROBAR UN PROYECTO AGL  PARA LA  CANCELACIÓN  DE LOS EXÁMENES DE LABORATORIO  O LA RECONVERSIÓN DE RECURSOS , YA SEA RENDIR  RECURSO HUMANO DE DOTACIÓN  MUNICIPAL DE SALUD Y PARA PODER CONTAR DE ESA MANERA CON  EL DINERO DISPONIBLE PARA LA CANCELACIÓN DEL LABORATOTRIO  U  OTRA VIA POSIBLE DE COLABORACIÓN.&lt;br /&gt;
-2.-  SE REQUIERE EL APOYO DEL MINISTERIO DE SALUD EN EL PROCESO DE ACREDITACIÓN EN CALIDAD, 20 MILLONES PARA LA INSCRIPCIÓN EN EL PROCESO Y MEJORAS INTERNAS QUE SE REQUIERAN REALIZAR EN POSTAS Y CESFAM PARA AFRONTAR DICHO PROCESO.&lt;br /&gt;
-3.- ADQUISICIÓN DE CAMIONETA PARA RONDAS ASISITENCIALES Y OTRAS PRESTACIONES.&lt;br /&gt;
-4.- APROBACIÓN DE AGL Y PMI&lt;br /&gt;
-5.- CANCELACIÓN DE RECURSO HUMANO DE DOTACIÓN PARA LIBERACIÓN DE PRESUPUESTO&lt;br /&gt;
-&lt;br /&gt;
-                                                             AGRADECIDOS DEL APOYO.</t>
-        </is>
-      </c>
-      <c r="K148" t="inlineStr">
-        <is>
-          <t>Mildred Varela</t>
-        </is>
-      </c>
-      <c r="L148" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M148" t="inlineStr">
-        <is>
-          <t>MUNICIPALIDAD DE PAIHUANO</t>
-        </is>
-      </c>
-      <c r="N148" t="inlineStr">
-        <is>
-          <t>ILUSTRE MUNICIPALIDAD DE PAIHUANO</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800576</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>AO001AW1825815</t>
-        </is>
-      </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>2025-05-12 09:30:00-04</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>lo recibirá en audiencia Alyson Morales Asesora del Gabinete 
- Via TEEMUnirse a la reunión ahora 
-Id. de reunión: 264 303 737 002 5 
-Código de acceso: De6hw7fe</t>
-        </is>
-      </c>
-      <c r="H149" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J149" t="inlineStr">
-        <is>
-          <t>Presentar los Círculos de Escucha como una tecnología social y práctica grupal de bienestar recogida en el REM, y a Corporación Escuchar, como OSFL con 10 años de experiencia en instalar Círculos de Escucha y formar monitoras/es para ello. &lt;br /&gt;
-Proponemos usar Círculos de Escucha para:&lt;br /&gt;
-- promover la participación ciudadana en salud.&lt;br /&gt;
-- promover bienestar y salud comunitaria a bajo costo, en base a la comunidad.&lt;br /&gt;
-- construir y/o desarrollar vínculos saludables para potenciar las comunidades.&lt;br /&gt;
-- levantar, relevar, difundir y potenciar los activos comunitarios territoriales.</t>
-        </is>
-      </c>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>Verónica Virgilio</t>
-        </is>
-      </c>
-      <c r="L149" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M149" t="inlineStr"/>
-      <c r="N149" t="inlineStr">
-        <is>
-          <t>Corporación Escuchar</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr"/>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
-      <c r="D150" t="inlineStr"/>
-      <c r="E150" t="inlineStr"/>
-      <c r="F150" t="inlineStr"/>
-      <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
-      <c r="J150" t="inlineStr"/>
-      <c r="K150" t="inlineStr">
-        <is>
-          <t>Yasna Nanjari</t>
-        </is>
-      </c>
-      <c r="L150" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M150" t="inlineStr"/>
-      <c r="N150" t="inlineStr">
-        <is>
-          <t>Corporación Escuchar</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/800572</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>AO001AW1815203</t>
-        </is>
-      </c>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>2025-05-09 11:00:00-04</t>
-        </is>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>lo recibirá en reunión  Alyson Morales asesora del Gabinete  por TEEM
-Microsoft Teams 
-Unirse a la reunión ahora 
-Id. de reunión: 285 804 262 906 4 
-Código de acceso: ch7HJ6qQ</t>
-        </is>
-      </c>
-      <c r="H151" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J151" t="inlineStr">
-        <is>
-          <t>Vulneración de derechos a paciente Albero Jesús Garrido Pérez, en atenciones brindadas.</t>
-        </is>
-      </c>
-      <c r="K151" t="inlineStr">
-        <is>
-          <t>Alberto Garrido</t>
-        </is>
-      </c>
-      <c r="L151" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M151" t="inlineStr"/>
-      <c r="N151" t="inlineStr">
-        <is>
-          <t>Gabriela Calderón Álvarez</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/796230</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>AO001AW1822942</t>
-        </is>
-      </c>
-      <c r="E152" t="inlineStr">
-        <is>
-          <t>2025-05-08 11:30:00-04</t>
-        </is>
-      </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t>Presencial</t>
-        </is>
-      </c>
-      <c r="G152" t="inlineStr">
-        <is>
-          <t>Mac Iver 541 piso 2 Ministerio de Salud, contacto Doris González 225740370</t>
-        </is>
-      </c>
-      <c r="H152" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J152" t="inlineStr">
-        <is>
-          <t>Presentar Exposalud 2025 a realizarse 1,2 y 3 de diciembre en Espacio Riesco, con la finalidad de mostrar la plataforma público privada que es y como es que esto favorece la comunicación en el área de Salud. Es necesario que sepa las gestiones que realizamos para contar con su acuerdo y verificar que nos aliniemos en el trabajo a realizar.</t>
-        </is>
-      </c>
-      <c r="K152" t="inlineStr">
-        <is>
-          <t>Andrea Buzzetti</t>
-        </is>
-      </c>
-      <c r="L152" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M152" t="inlineStr">
-        <is>
-          <t>FRESENIUS KABI</t>
-        </is>
-      </c>
-      <c r="N152" t="inlineStr">
-        <is>
-          <t>andrea buzzetti</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr"/>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-      <c r="D153" t="inlineStr"/>
-      <c r="E153" t="inlineStr"/>
-      <c r="F153" t="inlineStr"/>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
-      <c r="I153" t="inlineStr"/>
-      <c r="J153" t="inlineStr"/>
-      <c r="K153" t="inlineStr">
-        <is>
-          <t>Miguel Berrios Momberg</t>
-        </is>
-      </c>
-      <c r="L153" t="inlineStr">
-        <is>
-          <t>Gestor de intereses</t>
-        </is>
-      </c>
-      <c r="M153" t="inlineStr"/>
-      <c r="N153" t="inlineStr">
-        <is>
-          <t>Miguel Berrios</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/787881</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>AO001AW1822390</t>
-        </is>
-      </c>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>2025-04-25 10:00:00-04</t>
-        </is>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>se encomendó a la División de Inversiones lo recibió  Adrian Peña  25 abril</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J154" t="inlineStr">
         <is>
           <t>Señor&lt;br /&gt;
 &lt;br /&gt;
@@ -7804,81 +7229,602 @@
 Datamedica Spa.</t>
         </is>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Miguel Arteaga</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>Lobbista</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>DATAMEDICA S.A</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>DATAMEDICA SPA</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Bernardo Martorell</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Subsecretario de Redes Asistenciales</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/791214</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>AO001AW1813233</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2025-04-24 10:30:00-04</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>lo recibió  Alison Morales Asesora del Gabinete</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>Solicita audiencia Lobby para tratar situación actual del Centro Anun y todo lo que conlleva a su continuidad.</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>Carla Torres</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>municipalidad de Coronel</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Boris CHAMORRO</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Paola Pontoni</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Jefa Departamento de Reducción del Riesgo para Emergencias Sanitarias - SSP</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/257591/805327</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>AO001AW1854499</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>2025-06-09 04:30:00-04</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Monjitas 689 piso 7 oficina 72</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Soy medico urgenciologo, magister en emergencia y desastres. Me gustaría la asesoría de la jefa de departamento para el diseño de un proyecto que estoy llevando a cabo sobre manejo de múltiples victimas en hospitales.</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>Rubén Nissin</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>ruben nissin</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Paola Pontoni</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Jefa Departamento de Reducción del Riesgo para Emergencias Sanitarias - SSP</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/257591/805541</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>AO001AW1815597</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:30:00-04</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>oficina 1001 monjitas 565</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>Oportunidades de Mercado para la gestión climática bajo Art 6 del Acuerdo de París:&lt;br /&gt;
+(1) lista priorizada para tipología de proyectos; (2) línea del tiempo para lista priorizada; (3) apetito de proyectos en sector</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>María Lucila Serra Lahunsembarne</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>South Pole Carbon Asset Management Ltd.</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>South Pole Carbon Asset Management Ltd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>Rodrigo Bórquez</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>South Pole Carbon Asset Management Ltd.</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>South Pole Carbon Asset Management Ltd.</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Edith Carmen Ortiz Nuñez</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/786768</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>AO001AW1828916</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>2025-04-17 10:30:00-04</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>On line</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>Presentación de productos para detección y categorización de VPH, detección de VIH, Sífilis, HCV y HTLV&lt;br /&gt;
+&lt;br /&gt;
+Presentan equipos e insumos para la autotoma de examen de detección de VPH, a través de orina, permitiendo la amplificación y secuenciación de algunos genotipos. Presentan equipos e insumos para otros agentes: VIH, VHC, HTLV1, Sífilis. &lt;br /&gt;
+&lt;br /&gt;
+Se les sugiere reunión con ANACAN, y con redes asistenciales.&lt;br /&gt;
+&lt;br /&gt;
+Participan&lt;br /&gt;
+Dr. Leonardo Chanqueo Cornejo&lt;br /&gt;
+Carolina Peredo Courtier</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>Andrés Fernández</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>Sociedad Comercial Mihovilovic Hnos. y Otro Ltda.</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>Sociedad Comercial Mihovilovic y Hnos y otro Limitada</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>Jorge Touma</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>Sociedad Comercial Mihovilovic Hnos. y Otro Ltda.</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>Sociedad Comercial Mihovilovic y Hnos y otro Limitada</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Edith Carmen Ortiz Nuñez</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/787885</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>AO001AW1776471</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>2025-02-06 14:30:00-03</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>On line</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>Reunión de seguimiento lobby AO001AW1749073 en relación a la situación de Kaletra jarabe en programa VIH y una posible descontinuación.&lt;br /&gt;
+&lt;br /&gt;
+Se informa que se consultó al Comité asesor VIH pediátrico sobre existencia de alternativas terapéuticas, quienes señalaron y manifestaron la necesidad de mantener la disponibilidad de Kaletra® jarabe como parte del arsenal farmacológico para los niños y niñas que viven con VIH. &lt;br /&gt;
+Las alternativas disponibles en nuestro país pueden utilizarse a partir de los 40 kg, siendo inapropiados para la mayoría de los niños en crecimiento y no disponemos en Chile de su formulación en jarabes. Actualmente existen niños en control en que Kaletra® jarabe forma parte de su esquema de 2da línea y que no tienen el peso adecuado para optar a las alternativas disponibles.  &lt;br /&gt;
+&lt;br /&gt;
+Señalan que con estos antecedentes y teniendo claridad del requerimiento desde MINSAL realizarán gestiones para mantener la provisión de este producto en el país. &lt;br /&gt;
+&lt;br /&gt;
+Desde MINSAL se solicita informar sobre los avances de las gestiones por lo que se acuerda realizar una próxima reunión de seguimiento. &lt;br /&gt;
+ &lt;br /&gt;
+Participan&lt;br /&gt;
+Leonardo Chanqueo Cornejo&lt;br /&gt;
+María Teresa Silva</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>María Pons</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>Abbvie Ltda</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>Claudio Silva</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>Abbvie Ltda</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Edith Carmen Ortiz Nuñez</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Jefa (S) Departamento Programa Nacional de Prevención y Control del VIH/SIDA e ITS DIPRECE</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/275447/780151</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>AO001AW1749073</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2025-01-22 12:30:00-03</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Oficina Programa de VIH</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>1 horas, 0 minutos</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Elaboración, dictación, modificación, denegación o rechazo de actos administrativos, proyectos de ley y leyes y también de las decisiones que tomen los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>Situación lopinavir/ritonavir solución oral en programa pediátrico VIH&lt;br /&gt;
+&lt;br /&gt;
+Señalan que debido a nuevas alternativas terapéuticas ha disminuido su demanda a nivel mundial, lo que se ha traducido en una discontinuación en la producción del producto. &lt;br /&gt;
+Actualmente tiene contrato vigente con CENABAST hasta diciembre 2025. Para el 2026 existe riesgo de descontinuación. &lt;br /&gt;
+Señalan que en caso de que MINSAL requiera mantener disponible este producto en el país podrían hacer las gestiones pertinentes para ello, considerando las dificultades que se pueden presentar. &lt;br /&gt;
+Desde el Depto VIH se plantea que es necesario disponer de esta presentación como una alternativa en tratamiento de rescate cuando existe resistencia a antirretrovirales. Lopinavir/ritonavir es la única alternativa que existe para estos casos en niños menores a &lt; 40 kilos. Igualmente se hará la consulta al Comité asesor VIH pediátrico para tener certeza que no existen otras alternativas terapéuticas en esta situación.&lt;br /&gt;
+Se acuerda realizar una próxima reunión de seguimiento para informar si se requiere mantener la disponibilidad de lopinavir/ritonavir solución en el país y realizar las gestiones correspondientes para ello. &lt;br /&gt;
+&lt;br /&gt;
+Asisten&lt;br /&gt;
+&lt;br /&gt;
+Dr. leonardo Chanqueo   Jefe Programa de VIH&lt;br /&gt;
+Sra. María Teresa Silva Profesional Programa de VIH&lt;br /&gt;
+Sra. María Pons&lt;br /&gt;
+Sr. Claudio Silva</t>
+        </is>
+      </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>Miguel Arteaga</t>
+          <t>María Pons</t>
         </is>
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>Lobista</t>
-        </is>
-      </c>
-      <c r="M154" t="inlineStr">
-        <is>
-          <t>DATAMEDICA S.A</t>
-        </is>
-      </c>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr"/>
       <c r="N154" t="inlineStr">
         <is>
-          <t>DATAMEDICA SPA</t>
+          <t>Abbvie Ltda</t>
         </is>
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Bernardo Martorell</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>Subsecretario de Redes Asistenciales</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/791073/791214</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>AO001AW1813233</t>
-        </is>
-      </c>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>2025-04-24 10:30:00-04</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>Videoconferencia</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>lo recibió  Alison Morales Asesora del Gabinete</t>
-        </is>
-      </c>
-      <c r="H155" t="inlineStr">
-        <is>
-          <t>1 horas, 0 minutos</t>
-        </is>
-      </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
-        </is>
-      </c>
-      <c r="J155" t="inlineStr">
-        <is>
-          <t>Solicita audiencia Lobby para tratar situación actual del Centro Anun y todo lo que conlleva a su continuidad.</t>
-        </is>
-      </c>
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
       <c r="K155" t="inlineStr">
         <is>
-          <t>Carla Torres</t>
+          <t>Claudio Silva</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
@@ -7889,29 +7835,83 @@
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr">
         <is>
-          <t>municipalidad de Coronel</t>
+          <t>Abbvie Ltda</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr"/>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
-      <c r="F156" t="inlineStr"/>
-      <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="inlineStr"/>
-      <c r="J156" t="inlineStr"/>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Carolina Neira</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Jefa (S) Departamento Enfermedades No Transmisibles</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://www.leylobby.gob.cl/instituciones/AO001/audiencias/2025/278283/792465</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>AO001AW1794134</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2025-05-09 15:00:00-04</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Videoconferencia</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>________________________________________________________________________________
+Microsoft Teams ¿Necesita ayuda? 
+Unirse a la reunión ahora 
+Id. de reunión: 228 396 235 533 1 
+Código de acceso: 5Nk3zg7Q 
+________________________________________</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>0 horas, 15 minutos</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>Celebración, modificación o terminación a cualquier título, de contratos que realicen los sujetos pasivos y que sean necesarios para su funcionamiento., 
+Diseño, implementación y evaluación de políticas, planes y programas efectuados por los sujetos pasivos.</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>No se presenta a audiencia de Lobby.</t>
+        </is>
+      </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>Boris CHAMORRO</t>
-        </is>
-      </c>
-      <c r="L156" t="inlineStr"/>
+          <t>Juan Ríos</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>Gestor de intereses</t>
+        </is>
+      </c>
       <c r="M156" t="inlineStr"/>
-      <c r="N156" t="inlineStr"/>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>Marcela Cofré Cervera</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -10041,7 +10041,7 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M206" t="inlineStr">
@@ -12378,7 +12378,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M252" t="inlineStr">
@@ -14661,7 +14661,7 @@
       </c>
       <c r="L301" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M301" t="inlineStr">
@@ -17744,7 +17744,7 @@
       </c>
       <c r="L360" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M360" t="inlineStr">
@@ -18612,7 +18612,7 @@
       </c>
       <c r="L380" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M380" t="inlineStr">
@@ -27202,7 +27202,7 @@
       </c>
       <c r="L540" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M540" t="inlineStr">
@@ -27653,7 +27653,7 @@
       </c>
       <c r="L551" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M551" t="inlineStr">
@@ -30845,7 +30845,7 @@
       </c>
       <c r="L621" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M621" t="inlineStr"/>
@@ -33530,7 +33530,7 @@
       </c>
       <c r="L681" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M681" t="inlineStr">
@@ -36415,7 +36415,7 @@
       </c>
       <c r="L739" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M739" t="inlineStr">
@@ -36820,7 +36820,7 @@
       </c>
       <c r="L747" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Gestor de intereses</t>
         </is>
       </c>
       <c r="M747" t="inlineStr">
@@ -37804,7 +37804,7 @@
       </c>
       <c r="L770" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M770" t="inlineStr">
@@ -39767,7 +39767,7 @@
       </c>
       <c r="L811" t="inlineStr">
         <is>
-          <t>Gestor de intereses</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M811" t="inlineStr">
@@ -45415,7 +45415,7 @@
       </c>
       <c r="L934" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M934" t="inlineStr">
@@ -45479,7 +45479,7 @@
       </c>
       <c r="L936" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M936" t="inlineStr">
@@ -46937,7 +46937,7 @@
       </c>
       <c r="L963" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M963" t="inlineStr">
@@ -47994,7 +47994,7 @@
       </c>
       <c r="L983" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M983" t="inlineStr"/>
@@ -48149,7 +48149,7 @@
       </c>
       <c r="L985" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M985" t="inlineStr">
@@ -48213,7 +48213,7 @@
       </c>
       <c r="L987" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M987" t="inlineStr">
@@ -48325,7 +48325,7 @@
       </c>
       <c r="L989" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M989" t="inlineStr">
@@ -48389,7 +48389,7 @@
       </c>
       <c r="L991" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M991" t="inlineStr">
@@ -49583,7 +49583,7 @@
       </c>
       <c r="L1011" t="inlineStr">
         <is>
-          <t>Lobista</t>
+          <t>Lobbista</t>
         </is>
       </c>
       <c r="M1011" t="inlineStr">

</xml_diff>